<commit_message>
New line chart embedded for declining manual efforts
</commit_message>
<xml_diff>
--- a/Test Automation Estimation, Delivery Planner and ROI Calculator - Template.xlsx
+++ b/Test Automation Estimation, Delivery Planner and ROI Calculator - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReusableComponents\roi-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26BC271-224D-4527-9B77-4CB6D68346CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19214653-B2D9-42FE-9155-1A0588936036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="778" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="778" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputParameters" sheetId="16" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -110,18 +110,12 @@
     <t>S12</t>
   </si>
   <si>
-    <t>S13</t>
-  </si>
-  <si>
     <t>Sprint</t>
   </si>
   <si>
     <t>Automated TCs</t>
   </si>
   <si>
-    <t>S14</t>
-  </si>
-  <si>
     <t>Complexity</t>
   </si>
   <si>
@@ -137,16 +131,10 @@
     <t>Total ROI Per TC</t>
   </si>
   <si>
-    <t>S15</t>
-  </si>
-  <si>
     <t>Capacity Per Day (Hrs)</t>
   </si>
   <si>
     <t>Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Sprint Week 0</t>
@@ -335,17 +323,23 @@
     <t>Expected Throughput Per Sprint (Considering 2 weeks Sprint + All Engineers)</t>
   </si>
   <si>
-    <t>ROI (Hrs/Exec | Cumulative)</t>
-  </si>
-  <si>
     <t>ROI (PDs/Exec|Cumulative)</t>
+  </si>
+  <si>
+    <t>Manual Efforts(Hrs)</t>
+  </si>
+  <si>
+    <t>ROI (Hrs/Exec)</t>
+  </si>
+  <si>
+    <t>Cumulative ROI (Hrs/Exec)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,12 +440,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -528,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -583,15 +571,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -705,20 +684,11 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -729,24 +699,33 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -894,9 +873,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'TC Development Plan + ROI '!$B$4:$B$18</c:f>
+              <c:f>'TC Development Plan + ROI '!$B$4:$B$15</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>S1</c:v>
                 </c:pt>
@@ -932,25 +911,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>S12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>S13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>S14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>S15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TC Development Plan + ROI '!$C$4:$C$18</c:f>
+              <c:f>'TC Development Plan + ROI '!$C$4:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>450</c:v>
                 </c:pt>
@@ -985,15 +955,6 @@
                   <c:v>33.333333333333201</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1031,9 +992,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'TC Development Plan + ROI '!$B$4:$B$18</c:f>
+              <c:f>'TC Development Plan + ROI '!$B$4:$B$15</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>S1</c:v>
                 </c:pt>
@@ -1069,25 +1030,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>S12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>S13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>S14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>S15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TC Development Plan + ROI '!$D$4:$D$18</c:f>
+              <c:f>'TC Development Plan + ROI '!$D$4:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1122,15 +1074,6 @@
                   <c:v>416.6666666666668</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>450</c:v>
                 </c:pt>
               </c:numCache>
@@ -1158,15 +1101,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TC Development Plan + ROI '!$F$3</c:f>
+              <c:f>'TC Development Plan + ROI '!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ROI (PDs/Exec|Cumulative)</c:v>
+                  <c:v>ROI (Hrs/Exec)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1174,9 +1117,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
+              <a:tailEnd type="arrow"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1185,9 +1129,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'TC Development Plan + ROI '!$B$4:$B$18</c:f>
+              <c:f>'TC Development Plan + ROI '!$B$4:$B$15</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>S1</c:v>
                 </c:pt>
@@ -1223,69 +1167,174 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>S12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>S13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>S14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>S15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TC Development Plan + ROI '!$F$4:$F$18</c:f>
+              <c:f>'TC Development Plan + ROI '!$E$4:$E$15</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.166666666666667</c:v>
+                  <c:v>33.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3333333333333339</c:v>
+                  <c:v>66.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.500000000000002</c:v>
+                  <c:v>100.00000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.666666666666668</c:v>
+                  <c:v>133.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.833333333333339</c:v>
+                  <c:v>166.66666666666671</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.000000000000007</c:v>
+                  <c:v>200.00000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.166666666666675</c:v>
+                  <c:v>233.3333333333334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.333333333333343</c:v>
+                  <c:v>266.66666666666674</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.500000000000014</c:v>
+                  <c:v>300.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41.666666666666686</c:v>
+                  <c:v>333.33333333333348</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>86.666666666666686</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>131.66666666666669</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>176.66666666666669</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>221.66666666666669</c:v>
+                  <c:v>360</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-21CB-41DE-88A3-A6FC4152339D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TC Development Plan + ROI '!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manual Efforts(Hrs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+              <a:tailEnd type="oval"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TC Development Plan + ROI '!$B$4:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>S1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>S2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>S4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>S8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>S9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>S10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>S12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TC Development Plan + ROI '!$H$4:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>326.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>293.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>260.00000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226.66666666666671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>193.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160.00000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>126.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,7 +1342,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-21CB-41DE-88A3-A6FC4152339D}"/>
+              <c16:uniqueId val="{00000000-8EFF-4EED-8EE4-D4FA3B205D01}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1313,21 +1362,21 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
+                <c:idx val="3"/>
+                <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'TC Development Plan + ROI '!$E$3</c15:sqref>
+                          <c15:sqref>'TC Development Plan + ROI '!$G$3</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>ROI (Hrs/Exec | Cumulative)</c:v>
+                        <c:v>ROI (PDs/Exec|Cumulative)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1335,7 +1384,7 @@
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent3"/>
+                      <a:schemeClr val="accent4"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -1349,12 +1398,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'TC Development Plan + ROI '!$B$4:$B$18</c15:sqref>
+                          <c15:sqref>'TC Development Plan + ROI '!$B$4:$B$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0">
                         <c:v>S1</c:v>
                       </c:pt>
@@ -1391,15 +1440,6 @@
                       <c:pt idx="11">
                         <c:v>S12</c:v>
                       </c:pt>
-                      <c:pt idx="12">
-                        <c:v>S13</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>S14</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>S15</c:v>
-                      </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
@@ -1408,57 +1448,48 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'TC Development Plan + ROI '!$E$4:$E$18</c15:sqref>
+                          <c15:sqref>'TC Development Plan + ROI '!$G$4:$G$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>0</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>33.333333333333336</c:v>
+                        <c:v>4.166666666666667</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>66.666666666666671</c:v>
+                        <c:v>12.5</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>100.00000000000001</c:v>
+                        <c:v>25</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>133.33333333333334</c:v>
+                        <c:v>41.666666666666671</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>166.66666666666671</c:v>
+                        <c:v>62.500000000000014</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>200.00000000000006</c:v>
+                        <c:v>87.500000000000028</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>233.3333333333334</c:v>
+                        <c:v>116.6666666666667</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>266.66666666666674</c:v>
+                        <c:v>150.00000000000006</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>300.00000000000011</c:v>
+                        <c:v>187.50000000000006</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>333.33333333333348</c:v>
+                        <c:v>229.16666666666674</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>693.33333333333348</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>1053.3333333333335</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>1413.3333333333335</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>1773.3333333333335</c:v>
+                        <c:v>274.16666666666674</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1466,7 +1497,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-21CB-41DE-88A3-A6FC4152339D}"/>
+                    <c16:uniqueId val="{00000003-21CB-41DE-88A3-A6FC4152339D}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1588,7 +1619,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1635,6 +1666,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1616849023"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1656,8 +1688,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.30060543582332305"/>
           <c:y val="6.9448182740155656E-2"/>
-          <c:w val="0.41947693560034538"/>
-          <c:h val="3.2538763831421832E-2"/>
+          <c:w val="0.40601049652373616"/>
+          <c:h val="2.9347774288592341E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2293,13 +2325,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1963</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>6414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>19639</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>9820</xdr:rowOff>
@@ -2608,7 +2640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6551093D-8E4B-4356-BA7E-0D2DD3C5E751}">
   <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2634,13 +2666,13 @@
       <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:8">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="F2" s="34" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G2" s="34"/>
       <c r="H2" s="30">
@@ -2649,14 +2681,14 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="26">
         <v>100</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="30">
@@ -2666,14 +2698,14 @@
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="26">
         <v>150</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G4" s="34"/>
       <c r="H4" s="32">
@@ -2682,7 +2714,7 @@
     </row>
     <row r="5" spans="2:8">
       <c r="B5" s="34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="26">
@@ -2690,10 +2722,10 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="24">
         <f>SUM(D3:D5)</f>
         <v>450</v>
@@ -2701,32 +2733,32 @@
     </row>
     <row r="7" spans="2:8"/>
     <row r="8" spans="2:8">
-      <c r="B8" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="43"/>
-      <c r="F8" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="43"/>
+      <c r="B8" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="F8" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>4</v>
@@ -2802,25 +2834,25 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="F13" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="37"/>
+      <c r="F13" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="42"/>
       <c r="H13" s="19">
         <f>SUM(H10:H12)</f>
         <v>1440</v>
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="F14" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="37"/>
+      <c r="B14" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="F14" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="42"/>
       <c r="H14" s="19">
         <f>H13+(H13*H4)</f>
         <v>1728</v>
@@ -2828,18 +2860,18 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="37"/>
+      <c r="F15" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="42"/>
       <c r="H15" s="19">
         <f>H14/8</f>
         <v>216</v>
@@ -2856,10 +2888,10 @@
         <f>C16*D10</f>
         <v>8100</v>
       </c>
-      <c r="F16" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="37"/>
+      <c r="F16" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="42"/>
       <c r="H16" s="19">
         <f>H15/(H3/8)</f>
         <v>108</v>
@@ -2891,7 +2923,7 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C19" s="35"/>
       <c r="D19" s="23">
@@ -2901,7 +2933,7 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="23">
@@ -2909,7 +2941,7 @@
         <v>360</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G20" s="35"/>
       <c r="H20" s="20">
@@ -2919,15 +2951,15 @@
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="23">
         <f>D20/8</f>
         <v>45</v>
       </c>
-      <c r="F21" s="50" t="s">
-        <v>87</v>
+      <c r="F21" s="37" t="s">
+        <v>83</v>
       </c>
       <c r="G21" s="35"/>
       <c r="H21" s="31">
@@ -2937,7 +2969,7 @@
     </row>
     <row r="22" spans="2:8">
       <c r="F22" s="35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G22" s="35"/>
       <c r="H22" s="20">
@@ -2946,16 +2978,16 @@
       </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="39"/>
+      <c r="B23" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="45"/>
       <c r="D23" s="33">
         <f>(D21*8)/D6</f>
         <v>0.8</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G23" s="35"/>
       <c r="H23" s="20">
@@ -2966,6 +2998,13 @@
     <row r="24" spans="2:8"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B20:C20"/>
@@ -2982,13 +3021,6 @@
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2998,10 +3030,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02538A64-B9C7-4D60-98BE-12062C4CF6CA}">
-  <dimension ref="A2:F21"/>
+  <dimension ref="B2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
@@ -3010,37 +3042,47 @@
     <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
-      <c r="B2" s="48" t="s">
+    <row r="2" spans="2:9">
+      <c r="B2" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
+        <v>87</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3054,17 +3096,25 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="6">
-        <f>E4/8</f>
+      <c r="F4" s="4">
+        <f>E4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="G4" s="6">
+        <f>F4/8</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <f>InputParameters!D23*InputParameters!D6</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C18" si="0">IF($C$4-D5&gt;$C$4,$C$4,$C$4-D5)</f>
+        <f t="shared" ref="C5:C15" si="0">IF($C$4-D5&gt;$C$4,$C$4,$C$4-D5)</f>
         <v>408.33333333333331</v>
       </c>
       <c r="D5" s="6">
@@ -3072,15 +3122,23 @@
         <v>41.666666666666671</v>
       </c>
       <c r="E5" s="4">
-        <f>IF(D5&gt;=$C$4,(D5*InputParameters!$D$23)+E4,D5*InputParameters!$D$23)</f>
+        <f>IF(D5&gt;=$C$4,(D5*InputParameters!$D$23),D5*InputParameters!$D$23)</f>
         <v>33.333333333333336</v>
       </c>
-      <c r="F5" s="6">
-        <f t="shared" ref="F5:F16" si="1">E5/8</f>
+      <c r="F5" s="4">
+        <f>E5+F4</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="G5" s="6">
+        <f>F5/8</f>
         <v>4.166666666666667</v>
       </c>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="H5" s="4">
+        <f>IF(H4-$E$5&lt;0,0,H4-$E$5)</f>
+        <v>326.66666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3093,15 +3151,24 @@
         <v>83.333333333333343</v>
       </c>
       <c r="E6" s="4">
-        <f>IF(D6&gt;=$C$4,(D6*InputParameters!$D$23)+E5,D6*InputParameters!$D$23)</f>
+        <f>IF(D6&gt;=$C$4,(D6*InputParameters!$D$23),D6*InputParameters!$D$23)</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="F6" s="6">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333339</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="F6" s="4">
+        <f>E6+F5</f>
+        <v>100</v>
+      </c>
+      <c r="G6" s="6">
+        <f>F6/8</f>
+        <v>12.5</v>
+      </c>
+      <c r="H6" s="4">
+        <f>IF(H5-$E$5&lt;0,0,H5-$E$5)</f>
+        <v>293.33333333333337</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -3114,15 +3181,24 @@
         <v>125.00000000000001</v>
       </c>
       <c r="E7" s="4">
-        <f>IF(D7&gt;=$C$4,(D7*InputParameters!$D$23)+E6,D7*InputParameters!$D$23)</f>
+        <f>IF(D7&gt;=$C$4,(D7*InputParameters!$D$23),D7*InputParameters!$D$23)</f>
         <v>100.00000000000001</v>
       </c>
-      <c r="F7" s="6">
-        <f t="shared" si="1"/>
-        <v>12.500000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="F7" s="4">
+        <f>E7+F6</f>
+        <v>200</v>
+      </c>
+      <c r="G7" s="6">
+        <f>F7/8</f>
+        <v>25</v>
+      </c>
+      <c r="H7" s="4">
+        <f>IF(H6-$E$5&lt;0,0,H6-$E$5)</f>
+        <v>260.00000000000006</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -3135,15 +3211,23 @@
         <v>166.66666666666669</v>
       </c>
       <c r="E8" s="4">
-        <f>IF(D8&gt;=$C$4,(D8*InputParameters!$D$23)+E7,D8*InputParameters!$D$23)</f>
+        <f>IF(D8&gt;=$C$4,(D8*InputParameters!$D$23),D8*InputParameters!$D$23)</f>
         <v>133.33333333333334</v>
       </c>
-      <c r="F8" s="6">
-        <f t="shared" si="1"/>
-        <v>16.666666666666668</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="F8" s="4">
+        <f>E8+F7</f>
+        <v>333.33333333333337</v>
+      </c>
+      <c r="G8" s="6">
+        <f>F8/8</f>
+        <v>41.666666666666671</v>
+      </c>
+      <c r="H8" s="4">
+        <f>IF(H7-$E$5&lt;0,0,H7-$E$5)</f>
+        <v>226.66666666666671</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
@@ -3156,15 +3240,23 @@
         <v>208.33333333333337</v>
       </c>
       <c r="E9" s="4">
-        <f>IF(D9&gt;=$C$4,(D9*InputParameters!$D$23)+E8,D9*InputParameters!$D$23)</f>
+        <f>IF(D9&gt;=$C$4,(D9*InputParameters!$D$23),D9*InputParameters!$D$23)</f>
         <v>166.66666666666671</v>
       </c>
-      <c r="F9" s="6">
-        <f t="shared" si="1"/>
-        <v>20.833333333333339</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="F9" s="4">
+        <f>E9+F8</f>
+        <v>500.00000000000011</v>
+      </c>
+      <c r="G9" s="6">
+        <f>F9/8</f>
+        <v>62.500000000000014</v>
+      </c>
+      <c r="H9" s="4">
+        <f>IF(H8-$E$5&lt;0,0,H8-$E$5)</f>
+        <v>193.33333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -3177,15 +3269,23 @@
         <v>250.00000000000006</v>
       </c>
       <c r="E10" s="4">
-        <f>IF(D10&gt;=$C$4,(D10*InputParameters!$D$23)+E9,D10*InputParameters!$D$23)</f>
+        <f>IF(D10&gt;=$C$4,(D10*InputParameters!$D$23),D10*InputParameters!$D$23)</f>
         <v>200.00000000000006</v>
       </c>
-      <c r="F10" s="6">
-        <f t="shared" si="1"/>
-        <v>25.000000000000007</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="F10" s="4">
+        <f>E10+F9</f>
+        <v>700.00000000000023</v>
+      </c>
+      <c r="G10" s="6">
+        <f>F10/8</f>
+        <v>87.500000000000028</v>
+      </c>
+      <c r="H10" s="4">
+        <f>IF(H9-$E$5&lt;0,0,H9-$E$5)</f>
+        <v>160.00000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
@@ -3198,15 +3298,23 @@
         <v>291.66666666666674</v>
       </c>
       <c r="E11" s="4">
-        <f>IF(D11&gt;=$C$4,(D11*InputParameters!$D$23)+E10,D11*InputParameters!$D$23)</f>
+        <f>IF(D11&gt;=$C$4,(D11*InputParameters!$D$23),D11*InputParameters!$D$23)</f>
         <v>233.3333333333334</v>
       </c>
-      <c r="F11" s="6">
-        <f t="shared" si="1"/>
-        <v>29.166666666666675</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="F11" s="4">
+        <f>E11+F10</f>
+        <v>933.3333333333336</v>
+      </c>
+      <c r="G11" s="6">
+        <f>F11/8</f>
+        <v>116.6666666666667</v>
+      </c>
+      <c r="H11" s="4">
+        <f>IF(H10-$E$5&lt;0,0,H10-$E$5)</f>
+        <v>126.66666666666669</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
@@ -3219,15 +3327,23 @@
         <v>333.33333333333343</v>
       </c>
       <c r="E12" s="4">
-        <f>IF(D12&gt;=$C$4,(D12*InputParameters!$D$23)+E11,D12*InputParameters!$D$23)</f>
+        <f>IF(D12&gt;=$C$4,(D12*InputParameters!$D$23),D12*InputParameters!$D$23)</f>
         <v>266.66666666666674</v>
       </c>
-      <c r="F12" s="6">
-        <f t="shared" si="1"/>
-        <v>33.333333333333343</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
+      <c r="F12" s="4">
+        <f>E12+F11</f>
+        <v>1200.0000000000005</v>
+      </c>
+      <c r="G12" s="6">
+        <f>F12/8</f>
+        <v>150.00000000000006</v>
+      </c>
+      <c r="H12" s="4">
+        <f>IF(H11-$E$5&lt;0,0,H11-$E$5)</f>
+        <v>93.333333333333343</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -3240,15 +3356,23 @@
         <v>375.00000000000011</v>
       </c>
       <c r="E13" s="4">
-        <f>IF(D13&gt;=$C$4,(D13*InputParameters!$D$23)+E12,D13*InputParameters!$D$23)</f>
+        <f>IF(D13&gt;=$C$4,(D13*InputParameters!$D$23),D13*InputParameters!$D$23)</f>
         <v>300.00000000000011</v>
       </c>
-      <c r="F13" s="6">
-        <f t="shared" si="1"/>
-        <v>37.500000000000014</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="F13" s="4">
+        <f>E13+F12</f>
+        <v>1500.0000000000005</v>
+      </c>
+      <c r="G13" s="6">
+        <f>F13/8</f>
+        <v>187.50000000000006</v>
+      </c>
+      <c r="H13" s="4">
+        <f>IF(H12-$E$5&lt;0,0,H12-$E$5)</f>
+        <v>60.000000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
@@ -3261,15 +3385,23 @@
         <v>416.6666666666668</v>
       </c>
       <c r="E14" s="4">
-        <f>IF(D14&gt;=$C$4,(D14*InputParameters!$D$23)+E13,D14*InputParameters!$D$23)</f>
+        <f>IF(D14&gt;=$C$4,(D14*InputParameters!$D$23),D14*InputParameters!$D$23)</f>
         <v>333.33333333333348</v>
       </c>
-      <c r="F14" s="6">
-        <f t="shared" si="1"/>
-        <v>41.666666666666686</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="F14" s="4">
+        <f>E14+F13</f>
+        <v>1833.3333333333339</v>
+      </c>
+      <c r="G14" s="6">
+        <f>F14/8</f>
+        <v>229.16666666666674</v>
+      </c>
+      <c r="H14" s="4">
+        <f>IF(H13-$E$5&lt;0,0,H13-$E$5)</f>
+        <v>26.666666666666671</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -3282,86 +3414,56 @@
         <v>450</v>
       </c>
       <c r="E15" s="4">
-        <f>IF(D15&gt;=$C$4,(D15*InputParameters!$D$23)+E14,D15*InputParameters!$D$23)</f>
-        <v>693.33333333333348</v>
-      </c>
-      <c r="F15" s="6">
-        <f t="shared" si="1"/>
-        <v>86.666666666666686</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" si="0"/>
+        <f>IF(D15&gt;=$C$4,(D15*InputParameters!$D$23),D15*InputParameters!$D$23)</f>
+        <v>360</v>
+      </c>
+      <c r="F15" s="4">
+        <f>E15+F14</f>
+        <v>2193.3333333333339</v>
+      </c>
+      <c r="G15" s="6">
+        <f>F15/8</f>
+        <v>274.16666666666674</v>
+      </c>
+      <c r="H15" s="4">
+        <f>IF(H14-$E$5&lt;0,0,H14-$E$5)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="6">
-        <f>IF(D15+InputParameters!$H$21&gt;$C$4,$C$4,D15+InputParameters!$H$21)</f>
-        <v>450</v>
-      </c>
-      <c r="E16" s="4">
-        <f>IF(D16&gt;=$C$4,(D16*InputParameters!$D$23)+E15,D16*InputParameters!$D$23)</f>
-        <v>1053.3333333333335</v>
-      </c>
-      <c r="F16" s="6">
-        <f t="shared" si="1"/>
-        <v>131.66666666666669</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="6">
-        <f>IF(D16+InputParameters!$H$21&gt;$C$4,$C$4,D16+InputParameters!$H$21)</f>
-        <v>450</v>
-      </c>
-      <c r="E17" s="4">
-        <f>IF(D17&gt;=$C$4,(D17*InputParameters!$D$23)+E16,D17*InputParameters!$D$23)</f>
-        <v>1413.3333333333335</v>
-      </c>
-      <c r="F17" s="6">
-        <f>(E17/8)</f>
-        <v>176.66666666666669</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="B18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="6">
-        <f>IF(D17+InputParameters!$H$21&gt;$C$4,$C$4,D17+InputParameters!$H$21)</f>
-        <v>450</v>
-      </c>
-      <c r="E18" s="4">
-        <f>IF(D18&gt;=$C$4,(D18*InputParameters!$D$23)+E17,D18*InputParameters!$D$23)</f>
-        <v>1773.3333333333335</v>
-      </c>
-      <c r="F18" s="6">
-        <f>(E18/8)</f>
-        <v>221.66666666666669</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="21" spans="2:8">
       <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3390,361 +3492,362 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="2:7">
+      <c r="B2" s="47"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47" t="s">
+      <c r="F2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
+      <c r="G2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="47"/>
-    </row>
-    <row r="2" spans="2:7">
-      <c r="B2" s="44"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="44" t="s">
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="47"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F3" s="47"/>
+      <c r="G3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="44" t="s">
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="47"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="47"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="47" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="44"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="10" t="s">
+      <c r="E5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="10" t="s">
+      <c r="G5" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="47"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="47"/>
+      <c r="G6" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="47"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="47"/>
+      <c r="G7" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="47"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="44"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="10" t="s">
+      <c r="F8" s="47"/>
+      <c r="G8" s="48"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="47"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="44"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="44" t="s">
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="47"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="44" t="s">
+      <c r="E10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="44"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="44"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="44"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="12" t="s">
+      <c r="G10" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="47"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="47"/>
+      <c r="G11" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="47"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="47"/>
+      <c r="G12" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="47"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="49"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="47"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="49"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="46"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="44"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="46"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="44"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="44" t="s">
+      <c r="D15" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="44" t="s">
+      <c r="E15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="44"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="44"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="44"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="45"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="44"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="44" t="s">
+      <c r="G15" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="47"/>
+      <c r="C16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="47"/>
+      <c r="E16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="47"/>
+      <c r="C17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D17" s="47"/>
+      <c r="E17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="47"/>
+      <c r="G17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="44" t="s">
+    </row>
+    <row r="18" spans="2:7" ht="29">
+      <c r="B18" s="47"/>
+      <c r="C18" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="44" t="s">
+      <c r="D18" s="47"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="47"/>
+      <c r="C19" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="44"/>
-      <c r="C16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="44"/>
-      <c r="C17" s="10" t="s">
+      <c r="D19" s="47"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="47"/>
+      <c r="C20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="10" t="s">
+      <c r="D20" s="47"/>
+      <c r="E20" s="16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="29">
-      <c r="B18" s="44"/>
-      <c r="C18" s="15" t="s">
+      <c r="F20" s="47"/>
+      <c r="G20" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="47"/>
+      <c r="C21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="44"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="15" t="s">
+      <c r="D21" s="47"/>
+      <c r="E21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="44"/>
-      <c r="C19" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="44"/>
-      <c r="C20" s="16" t="s">
+    <row r="22" spans="2:7">
+      <c r="B22" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="16" t="s">
+      <c r="C22" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="44"/>
-      <c r="C21" s="16" t="s">
+      <c r="D22" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="16" t="s">
+      <c r="E22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="44" t="s">
+      <c r="G22" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="10" t="s">
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="47"/>
+      <c r="C23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="47"/>
+      <c r="G23" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="44" t="s">
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="47"/>
+      <c r="C24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="47"/>
+      <c r="E24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="47"/>
+      <c r="G24" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="47"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="44" t="s">
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="47"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="15" t="s">
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="47"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="9" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="44"/>
-      <c r="C23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="44"/>
-      <c r="C24" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="44"/>
-      <c r="G24" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="44"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="44"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="44"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="D15:D21"/>
+    <mergeCell ref="F15:F21"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="E25:E27"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="D5:D9"/>
     <mergeCell ref="F5:F9"/>
@@ -3753,39 +3856,18 @@
     <mergeCell ref="D10:D14"/>
     <mergeCell ref="F10:F14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="D15:D21"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="F22:F27"/>
-    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="F2:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b8f8c10c-2db2-48d6-be80-a0b00d178529">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4b2faeb1-8c91-4335-966e-cc00e0900229" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EAAAF61DF58F5649BF3447A370204FFD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9758e6b5d890a198f89404ed33e1597">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b8f8c10c-2db2-48d6-be80-a0b00d178529" xmlns:ns3="4b2faeb1-8c91-4335-966e-cc00e0900229" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd80449eba01273d9a1ec4b941c1a1d1" ns2:_="" ns3:_="">
     <xsd:import namespace="b8f8c10c-2db2-48d6-be80-a0b00d178529"/>
@@ -4022,7 +4104,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b8f8c10c-2db2-48d6-be80-a0b00d178529">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4b2faeb1-8c91-4335-966e-cc00e0900229" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E5BC2FE-47EB-44B0-94DF-C123B859C6E1}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554E461D-632C-46D9-BCE1-300D8E3796F0}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{088F9AF3-CD7B-44E7-A596-BE57AE97905E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4037,16 +4151,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554E461D-632C-46D9-BCE1-300D8E3796F0}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E5BC2FE-47EB-44B0-94DF-C123B859C6E1}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>